<commit_message>
Homelessness NPA text correction
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -148,7 +148,7 @@
     <t xml:space="preserve">NPAH funded agencies were required to participate in the SHSC administered by the Australian Institute of Health and Welfare – although some were granted an exemption by the Commonwealth.</t>
   </si>
   <si>
-    <t xml:space="preserve">The SHSC does not report on NPAH initiatives exclusively, it also includes services funded under the National Affordable Housing Agreement.</t>
+    <t xml:space="preserve">Published SHSC data includes data from NPAH initiatives and services funded under NAHA.</t>
   </si>
   <si>
     <t xml:space="preserve">The number of initiatives delivered does not necessarily provide an indication of the scale, reach and effectiveness of services.</t>
@@ -322,7 +322,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -405,6 +405,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1500,7 +1504,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1573,9 +1577,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="21" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Homelessness text fixes. INdig NAPLAN fixes.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="45">
   <si>
     <t xml:space="preserve">Percentage of specialist homelessness services clients with needs met for accommodation and other services; and experiencing family and domestic violence, and young people (15-24 years old) presenting alone 2012-13 to 2016-17 </t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">The proportion of young people presenting alone as a proportion of all specialist homelessness services clients has decreased since 2012-13. However, clients experiencing family or domestic violence as a proportion of all specialist homelessness services clients has increased.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If there are increases in the proportion of people who have experienced domestic or family violence, or in young people presenting alone, this is most likely a reflection of increased need or from changes to services. These proportions could be expected to decrease in the long term as preventative strategies are implemented.</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -322,7 +319,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -400,10 +397,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1501,10 +1494,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,22 +1557,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="20" t="s">
+    <row r="8" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="19" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1588,19 +1581,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="B12" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>